<commit_message>
OP-465, Import test data updated and testing new database model.
</commit_message>
<xml_diff>
--- a/web/tellus_app/datasets/tellus_data/tests/fixture_files/metadata_aanvulling.xlsx
+++ b/web/tellus_app/datasets/tellus_data/tests/fixture_files/metadata_aanvulling.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="3260" yWindow="3480" windowWidth="30600" windowHeight="17400"/>
   </bookViews>
   <sheets>
     <sheet name="Locaties" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="173">
   <si>
     <r>
       <rPr>
@@ -27,6 +27,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Object nr.
 </t>
@@ -37,6 +38,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>(V&amp;OR)</t>
     </r>
@@ -48,6 +50,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Object nr.
 </t>
@@ -58,6 +61,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>(leverancier)</t>
     </r>
@@ -89,6 +93,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Rijksdriehoek
 </t>
@@ -99,6 +104,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> X-coördinaat (m)</t>
     </r>
@@ -110,6 +116,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Rijksdriehoek
 </t>
@@ -120,6 +127,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Y-coördinaat (m)</t>
     </r>
@@ -131,6 +139,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> WGS84 DD
 </t>
@@ -141,6 +150,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Latitude (gr)</t>
     </r>
@@ -152,6 +162,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> WGS84 DD
 </t>
@@ -162,6 +173,7 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Longitude (gr)</t>
     </r>
@@ -170,9 +182,6 @@
     <t>snelheidsklasse</t>
   </si>
   <si>
-    <t>meetlocatie (id)</t>
-  </si>
-  <si>
     <t>TP0001</t>
   </si>
   <si>
@@ -260,15 +269,9 @@
     <t>Oostoever</t>
   </si>
   <si>
-    <t>J Evertsenstraat</t>
-  </si>
-  <si>
     <t>Louvrelaan</t>
   </si>
   <si>
-    <t>Joh Huizingalaan</t>
-  </si>
-  <si>
     <t>TP0010</t>
   </si>
   <si>
@@ -314,15 +317,6 @@
     <t>AMSTD012</t>
   </si>
   <si>
-    <t>Hoofdweg 1 ri. JvGalenstr</t>
-  </si>
-  <si>
-    <t>J v Galenstraat</t>
-  </si>
-  <si>
-    <t>J Everstenstraat</t>
-  </si>
-  <si>
     <t>n.v.t.</t>
   </si>
   <si>
@@ -332,9 +326,6 @@
     <t>AMSTD013</t>
   </si>
   <si>
-    <t>Hoofdweg 2 ri. Mercatorpln.</t>
-  </si>
-  <si>
     <t>Mercatorplein</t>
   </si>
   <si>
@@ -344,274 +335,334 @@
     <t>AMSTD014</t>
   </si>
   <si>
+    <t>Op-/afrit A10 oostz.</t>
+  </si>
+  <si>
+    <t>JO Vaillantlaan</t>
+  </si>
+  <si>
+    <t>IJburg</t>
+  </si>
+  <si>
+    <t>Ring A10</t>
+  </si>
+  <si>
+    <t>TP0015</t>
+  </si>
+  <si>
+    <t>AMSTD015</t>
+  </si>
+  <si>
+    <t>Muiderlaan</t>
+  </si>
+  <si>
+    <t>Overdiemerweg</t>
+  </si>
+  <si>
+    <t>Muiden</t>
+  </si>
+  <si>
+    <t>TP0016</t>
+  </si>
+  <si>
+    <t>AMSTD016</t>
+  </si>
+  <si>
+    <t>Nieuwe Hemweg</t>
+  </si>
+  <si>
+    <t>Vlothavenweg</t>
+  </si>
+  <si>
+    <t>Centrum</t>
+  </si>
+  <si>
+    <t>Ring A 10</t>
+  </si>
+  <si>
+    <t>TP0017</t>
+  </si>
+  <si>
+    <t>AMSTD017</t>
+  </si>
+  <si>
+    <t>Kruislaan</t>
+  </si>
+  <si>
+    <t>Zaaiersweg</t>
+  </si>
+  <si>
+    <t>TP0018</t>
+  </si>
+  <si>
+    <t>AMSTD018</t>
+  </si>
+  <si>
+    <t>TP0019</t>
+  </si>
+  <si>
+    <t>AMSTD019</t>
+  </si>
+  <si>
+    <t>Karspeldreef</t>
+  </si>
+  <si>
+    <t>Flierbosdreef</t>
+  </si>
+  <si>
+    <t>Gooiseweg</t>
+  </si>
+  <si>
+    <t>TP0020</t>
+  </si>
+  <si>
+    <t>AMSTD020</t>
+  </si>
+  <si>
+    <t>Spaklerweg</t>
+  </si>
+  <si>
+    <t>Korte Ouderkerkerdijk</t>
+  </si>
+  <si>
+    <t>D Goedkoopstraat</t>
+  </si>
+  <si>
+    <t>TP0021</t>
+  </si>
+  <si>
+    <t>AMSTD021</t>
+  </si>
+  <si>
+    <t>J Franklinstraat</t>
+  </si>
+  <si>
+    <t>Admiralengracht</t>
+  </si>
+  <si>
+    <t>TP0022</t>
+  </si>
+  <si>
+    <t>AMSTD022</t>
+  </si>
+  <si>
+    <t>Hemsterhuisstraat</t>
+  </si>
+  <si>
+    <t>J Huizingalaan</t>
+  </si>
+  <si>
+    <t>TP0023</t>
+  </si>
+  <si>
+    <t>AMSTD023</t>
+  </si>
+  <si>
+    <t>Osdorp</t>
+  </si>
+  <si>
+    <t>TP0024</t>
+  </si>
+  <si>
+    <t>AMSTD024</t>
+  </si>
+  <si>
+    <t>Westeinde</t>
+  </si>
+  <si>
+    <t>Oosteinde</t>
+  </si>
+  <si>
+    <t>TP0025</t>
+  </si>
+  <si>
+    <t>AMSTD025</t>
+  </si>
+  <si>
+    <t>Van Diemenstraat</t>
+  </si>
+  <si>
+    <t>Van Neckstraat</t>
+  </si>
+  <si>
+    <t>Westerdoksdijk</t>
+  </si>
+  <si>
+    <t>TP0026</t>
+  </si>
+  <si>
+    <t>AMSTD026</t>
+  </si>
+  <si>
+    <t>Haarlemmerweg</t>
+  </si>
+  <si>
+    <t>Van Limburg Stirumstr.</t>
+  </si>
+  <si>
+    <t>Van der Duijnstraat</t>
+  </si>
+  <si>
+    <t>Nassauplein</t>
+  </si>
+  <si>
+    <t>Van Hallstraat</t>
+  </si>
+  <si>
+    <t>TP0027</t>
+  </si>
+  <si>
+    <t>AMSTD027</t>
+  </si>
+  <si>
+    <t>Bestevaerstraat</t>
+  </si>
+  <si>
+    <t>R Claeszenstraat</t>
+  </si>
+  <si>
+    <t>Adm. de Ruijterweg</t>
+  </si>
+  <si>
+    <t>W de Zwijgerlaan</t>
+  </si>
+  <si>
+    <t>TP0028</t>
+  </si>
+  <si>
+    <t>AMSTD028</t>
+  </si>
+  <si>
+    <t>IJ-tunnel</t>
+  </si>
+  <si>
+    <t>Joh.v Hasseltweg</t>
+  </si>
+  <si>
+    <t>Hagendoornplein</t>
+  </si>
+  <si>
+    <t>stad-uit (noord)</t>
+  </si>
+  <si>
+    <t>stad-in (zuid)</t>
+  </si>
+  <si>
+    <t>TP0029</t>
+  </si>
+  <si>
+    <t>AMSTD029</t>
+  </si>
+  <si>
+    <t>Klimopstraatje</t>
+  </si>
+  <si>
+    <t>Nieuwezijds Armsteeg</t>
+  </si>
+  <si>
+    <t>Raadhuisstraat</t>
+  </si>
+  <si>
+    <t>TP0030</t>
+  </si>
+  <si>
+    <t>AMSTD030</t>
+  </si>
+  <si>
+    <t>Prins Hendrikkade</t>
+  </si>
+  <si>
+    <t>TP0032</t>
+  </si>
+  <si>
+    <t>AMSTD032</t>
+  </si>
+  <si>
+    <t>Damrak</t>
+  </si>
+  <si>
+    <t>Oudebrugsteeg</t>
+  </si>
+  <si>
+    <t>TP0031</t>
+  </si>
+  <si>
+    <t>AMSTD031</t>
+  </si>
+  <si>
+    <t>Michiel de Ruytertunnel</t>
+  </si>
+  <si>
+    <t>Oostertoegang</t>
+  </si>
+  <si>
+    <t>Westertoegang</t>
+  </si>
+  <si>
+    <t>Westertoegang - Noordbuis</t>
+  </si>
+  <si>
+    <t>Oostertoegang - Zuidbuis</t>
+  </si>
+  <si>
+    <t>TP0033</t>
+  </si>
+  <si>
+    <t>Spaarndammertunnel</t>
+  </si>
+  <si>
+    <t>AMSTD033</t>
+  </si>
+  <si>
+    <t>TP0034</t>
+  </si>
+  <si>
+    <t>AMSTD034</t>
+  </si>
+  <si>
+    <t>Havikslaan</t>
+  </si>
+  <si>
+    <t>Hoofdweg</t>
+  </si>
+  <si>
+    <t>John Huizingalaan</t>
+  </si>
+  <si>
+    <t>Jan Evertsenstraat</t>
+  </si>
+  <si>
+    <t>Jan van Galenstraat</t>
+  </si>
+  <si>
+    <t>Jan Everstenstraat</t>
+  </si>
+  <si>
+    <t>Middenweg</t>
+  </si>
+  <si>
+    <t>Cornelis Lelylaan</t>
+  </si>
+  <si>
+    <t>Voorburgwal</t>
+  </si>
+  <si>
+    <t>Stadhouderskade</t>
+  </si>
+  <si>
     <t>IJburg 1 (IJburglaan)</t>
   </si>
   <si>
-    <t>Op-/afrit A10 oostz.</t>
-  </si>
-  <si>
-    <t>JO Vaillantlaan</t>
-  </si>
-  <si>
-    <t>IJburg</t>
-  </si>
-  <si>
-    <t>Ring A10</t>
-  </si>
-  <si>
-    <t>TP0015</t>
-  </si>
-  <si>
-    <t>AMSTD015</t>
-  </si>
-  <si>
     <t>IJburg 2 (W.Noordhoekkade)</t>
   </si>
   <si>
-    <t>Muiderlaan</t>
-  </si>
-  <si>
-    <t>Overdiemerweg</t>
-  </si>
-  <si>
-    <t>Muiden</t>
-  </si>
-  <si>
-    <t>TP0016</t>
-  </si>
-  <si>
-    <t>AMSTD016</t>
-  </si>
-  <si>
-    <t>Nieuwe Hemweg</t>
-  </si>
-  <si>
-    <t>Vlothavenweg</t>
-  </si>
-  <si>
-    <t>Centrum</t>
-  </si>
-  <si>
-    <t>Ring A 10</t>
-  </si>
-  <si>
-    <t>TP0017</t>
-  </si>
-  <si>
-    <t>AMSTD017</t>
-  </si>
-  <si>
-    <t>Middenweg ri. A10</t>
-  </si>
-  <si>
-    <t>Kruislaan</t>
-  </si>
-  <si>
-    <t>Zaaiersweg</t>
-  </si>
-  <si>
-    <t>TP0018</t>
-  </si>
-  <si>
-    <t>AMSTD018</t>
-  </si>
-  <si>
-    <t>Middenweg ri. Centrum</t>
-  </si>
-  <si>
-    <t>TP0019</t>
-  </si>
-  <si>
-    <t>AMSTD019</t>
-  </si>
-  <si>
-    <t>Karspeldreef</t>
-  </si>
-  <si>
-    <t>Flierbosdreef</t>
-  </si>
-  <si>
-    <t>Gooiseweg</t>
-  </si>
-  <si>
-    <t>TP0020</t>
-  </si>
-  <si>
-    <t>AMSTD020</t>
-  </si>
-  <si>
-    <t>Spaklerweg</t>
-  </si>
-  <si>
-    <t>Korte Ouderkerkerdijk</t>
-  </si>
-  <si>
-    <t>D Goedkoopstraat</t>
-  </si>
-  <si>
-    <t>TP0021</t>
-  </si>
-  <si>
-    <t>AMSTD021</t>
-  </si>
-  <si>
-    <t>Jan v Galenstraat-1</t>
-  </si>
-  <si>
-    <t>J Franklinstraat</t>
-  </si>
-  <si>
-    <t>Admiralengracht</t>
-  </si>
-  <si>
-    <t>TP0022</t>
-  </si>
-  <si>
-    <t>AMSTD022</t>
-  </si>
-  <si>
-    <t>Corn. Lelylaan ri. A10</t>
-  </si>
-  <si>
-    <t>Hemsterhuisstraat</t>
-  </si>
-  <si>
-    <t>J Huizingalaan</t>
-  </si>
-  <si>
-    <t>TP0023</t>
-  </si>
-  <si>
-    <t>AMSTD023</t>
-  </si>
-  <si>
-    <t>Corn. Lelylaan ri. Osdorp</t>
-  </si>
-  <si>
-    <t>Osdorp</t>
-  </si>
-  <si>
-    <t>TP0024</t>
-  </si>
-  <si>
-    <t>AMSTD024</t>
-  </si>
-  <si>
-    <t>Stadhouderskade-2</t>
-  </si>
-  <si>
-    <t>Westeinde</t>
-  </si>
-  <si>
-    <t>Oosteinde</t>
-  </si>
-  <si>
-    <t>TP0025</t>
-  </si>
-  <si>
-    <t>AMSTD025</t>
-  </si>
-  <si>
-    <t>Van Diemenstraat</t>
-  </si>
-  <si>
-    <t>Van Neckstraat</t>
-  </si>
-  <si>
-    <t>Westerdoksdijk</t>
-  </si>
-  <si>
-    <t>TP0026</t>
-  </si>
-  <si>
-    <t>AMSTD026</t>
-  </si>
-  <si>
-    <t>Haarlemmerweg</t>
-  </si>
-  <si>
-    <t>Van Limburg Stirumstr.</t>
-  </si>
-  <si>
-    <t>Van der Duijnstraat</t>
-  </si>
-  <si>
-    <t>Nassauplein</t>
-  </si>
-  <si>
-    <t>Van Hallstraat</t>
-  </si>
-  <si>
-    <t>TP0027</t>
-  </si>
-  <si>
-    <t>AMSTD027</t>
-  </si>
-  <si>
-    <t>Jan v Galenstraat-2</t>
-  </si>
-  <si>
-    <t>Bestevaerstraat</t>
-  </si>
-  <si>
-    <t>R Claeszenstraat</t>
-  </si>
-  <si>
-    <t>Adm. de Ruijterweg</t>
-  </si>
-  <si>
-    <t>W de Zwijgerlaan</t>
-  </si>
-  <si>
-    <t>TP0028</t>
-  </si>
-  <si>
-    <t>AMSTD028</t>
-  </si>
-  <si>
-    <t>IJ-tunnel</t>
-  </si>
-  <si>
-    <t>Joh.v Hasseltweg</t>
-  </si>
-  <si>
-    <t>Hagendoornplein</t>
-  </si>
-  <si>
-    <t>stad-uit (noord)</t>
-  </si>
-  <si>
-    <t>stad-in (zuid)</t>
-  </si>
-  <si>
-    <t>TP0029</t>
-  </si>
-  <si>
-    <t>AMSTD029</t>
-  </si>
-  <si>
-    <t>Voorburgwal-1</t>
-  </si>
-  <si>
-    <t>Klimopstraatje</t>
-  </si>
-  <si>
-    <t>Nieuwezijds Armsteeg</t>
-  </si>
-  <si>
-    <t>Raadhuisstraat</t>
-  </si>
-  <si>
-    <t>TP0030</t>
-  </si>
-  <si>
-    <t>AMSTD030</t>
-  </si>
-  <si>
-    <t>Voorburgwal-2</t>
-  </si>
-  <si>
-    <t>Prins Hendrikkade</t>
+    <t>meetlocatie id</t>
+  </si>
+  <si>
+    <t>Jan van Galenstraat 2</t>
+  </si>
+  <si>
+    <t>Jan van Galenstraat 1</t>
   </si>
 </sst>
 </file>
@@ -619,10 +670,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * #,##0.00\-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * #,##0.00\-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -639,12 +690,14 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -656,6 +709,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -693,6 +747,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -718,7 +784,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -778,15 +844,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -804,13 +900,65 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -835,11 +983,65 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="81">
     <cellStyle name="Euro" xfId="4"/>
     <cellStyle name="Euro 2" xfId="5"/>
     <cellStyle name="Euro 2 2" xfId="6"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
     <cellStyle name="Ongeldig 2" xfId="7"/>
     <cellStyle name="Ongeldig 3" xfId="8"/>
@@ -2050,10 +2252,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV27"/>
+  <dimension ref="A1:IV31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="14.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2069,7 +2271,7 @@
     <col min="9" max="9" width="14.83203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="1" customWidth="1"/>
     <col min="11" max="12" width="17.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" style="1" customWidth="1"/>
     <col min="14" max="256" width="9.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2111,30 +2313,30 @@
         <v>11</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="14.75" customHeight="1">
       <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="H2" s="6">
         <v>122475</v>
@@ -2157,24 +2359,24 @@
     </row>
     <row r="3" spans="1:13" ht="14.5" customHeight="1">
       <c r="A3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="F3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="9">
@@ -2198,25 +2400,25 @@
     </row>
     <row r="4" spans="1:13" ht="14.5" customHeight="1">
       <c r="A4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="H4" s="9">
         <v>122050</v>
@@ -2239,25 +2441,25 @@
     </row>
     <row r="5" spans="1:13" ht="14.5" customHeight="1">
       <c r="A5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="H5" s="9">
         <v>123765</v>
@@ -2280,25 +2482,25 @@
     </row>
     <row r="6" spans="1:13" ht="14.5" customHeight="1">
       <c r="A6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>43</v>
-      </c>
       <c r="F6" s="8" t="s">
-        <v>42</v>
+        <v>161</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>44</v>
+        <v>160</v>
       </c>
       <c r="H6" s="9">
         <v>117082</v>
@@ -2321,25 +2523,25 @@
     </row>
     <row r="7" spans="1:13" ht="14.5" customHeight="1">
       <c r="A7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="G7" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H7" s="9">
         <v>120590</v>
@@ -2362,25 +2564,25 @@
     </row>
     <row r="8" spans="1:13" ht="14.5" customHeight="1">
       <c r="A8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="G8" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="H8" s="9">
         <v>118905</v>
@@ -2403,25 +2605,25 @@
     </row>
     <row r="9" spans="1:13" ht="14.5" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>60</v>
+        <v>159</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>62</v>
+        <v>163</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H9" s="9">
         <v>118385</v>
@@ -2444,25 +2646,25 @@
     </row>
     <row r="10" spans="1:13" ht="14.5" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>66</v>
+        <v>159</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>62</v>
+        <v>163</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H10" s="9">
         <v>118385</v>
@@ -2480,30 +2682,30 @@
         <v>1</v>
       </c>
       <c r="M10" s="10">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="14.5" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>70</v>
+        <v>168</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H11" s="9">
         <v>127165</v>
@@ -2526,25 +2728,25 @@
     </row>
     <row r="12" spans="1:13" ht="14.5" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>77</v>
+        <v>169</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="H12" s="9">
         <v>129740</v>
@@ -2567,25 +2769,25 @@
     </row>
     <row r="13" spans="1:13" ht="14.5" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H13" s="9">
         <v>118995</v>
@@ -2608,25 +2810,25 @@
     </row>
     <row r="14" spans="1:13" ht="14.5" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>89</v>
+        <v>164</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H14" s="9">
         <v>124805</v>
@@ -2649,25 +2851,25 @@
     </row>
     <row r="15" spans="1:13" ht="14.5" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>94</v>
+        <v>164</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="H15" s="9">
         <v>124805</v>
@@ -2684,29 +2886,31 @@
       <c r="L15" s="9">
         <v>1</v>
       </c>
-      <c r="M15" s="10"/>
+      <c r="M15" s="10">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="14.5" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="H16" s="9">
         <v>126150</v>
@@ -2723,29 +2927,31 @@
       <c r="L16" s="9">
         <v>1</v>
       </c>
-      <c r="M16" s="10"/>
+      <c r="M16" s="10">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="1:13" ht="14.5" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="H17" s="9">
         <v>123190</v>
@@ -2762,29 +2968,31 @@
       <c r="L17" s="9">
         <v>1</v>
       </c>
-      <c r="M17" s="10"/>
+      <c r="M17" s="10">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="1:13" ht="14.5" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="H18" s="9">
         <v>116630</v>
@@ -2801,29 +3009,31 @@
       <c r="L18" s="9">
         <v>1</v>
       </c>
-      <c r="M18" s="10"/>
+      <c r="M18" s="10">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="1:13" ht="14.5" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>112</v>
+        <v>165</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H19" s="9">
         <v>118700</v>
@@ -2840,29 +3050,31 @@
       <c r="L19" s="9">
         <v>1</v>
       </c>
-      <c r="M19" s="10"/>
+      <c r="M19" s="10">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="1:13" ht="14.5" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>118</v>
+        <v>57</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="H20" s="9">
         <v>118700</v>
@@ -2879,29 +3091,31 @@
       <c r="L20" s="9">
         <v>1</v>
       </c>
-      <c r="M20" s="10"/>
+      <c r="M20" s="10">
+        <v>22</v>
+      </c>
     </row>
     <row r="21" spans="1:13" ht="14.5" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>121</v>
+        <v>167</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="H21" s="9">
         <v>121838.1</v>
@@ -2918,29 +3132,31 @@
       <c r="L21" s="9">
         <v>1</v>
       </c>
-      <c r="M21" s="10"/>
+      <c r="M21" s="10">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="1:13" ht="14.5" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H22" s="9">
         <v>121007.6</v>
@@ -2957,29 +3173,31 @@
       <c r="L22" s="9">
         <v>1</v>
       </c>
-      <c r="M22" s="10"/>
+      <c r="M22" s="10">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:13" ht="14.5" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="H23" s="9">
         <v>120176.8</v>
@@ -2996,29 +3214,31 @@
       <c r="L23" s="9">
         <v>1</v>
       </c>
-      <c r="M23" s="10"/>
+      <c r="M23" s="10">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="1:13" ht="14.5" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>138</v>
+        <v>171</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="H24" s="9">
         <v>119142.6</v>
@@ -3035,29 +3255,31 @@
       <c r="L24" s="9">
         <v>1</v>
       </c>
-      <c r="M24" s="10"/>
+      <c r="M24" s="10">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:13" ht="14.5" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="H25" s="9">
         <v>122575</v>
@@ -3074,29 +3296,31 @@
       <c r="L25" s="9">
         <v>1</v>
       </c>
-      <c r="M25" s="10"/>
+      <c r="M25" s="10">
+        <v>28</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="14.5" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H26" s="9">
         <v>121487</v>
@@ -3113,29 +3337,31 @@
       <c r="L26" s="9">
         <v>3</v>
       </c>
-      <c r="M26" s="11"/>
+      <c r="M26" s="11">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="1:13" ht="14.5" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>159</v>
+        <v>57</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>63</v>
+        <v>141</v>
       </c>
       <c r="H27" s="9">
         <v>121483</v>
@@ -3152,7 +3378,173 @@
       <c r="L27" s="9">
         <v>3</v>
       </c>
-      <c r="M27" s="11"/>
+      <c r="M27" s="11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="14.5" customHeight="1">
+      <c r="A28" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="H28" s="9">
+        <v>121981</v>
+      </c>
+      <c r="I28" s="9">
+        <v>488166</v>
+      </c>
+      <c r="J28" s="9">
+        <v>52.380369999999999</v>
+      </c>
+      <c r="K28" s="9">
+        <v>4.9022699999999997</v>
+      </c>
+      <c r="L28" s="9">
+        <v>1</v>
+      </c>
+      <c r="M28" s="12">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="14.75" customHeight="1">
+      <c r="A29" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" s="9">
+        <v>121626</v>
+      </c>
+      <c r="I29" s="9">
+        <v>487694</v>
+      </c>
+      <c r="J29" s="9">
+        <v>52.376100000000001</v>
+      </c>
+      <c r="K29" s="9">
+        <v>4.8971</v>
+      </c>
+      <c r="L29" s="9">
+        <v>1</v>
+      </c>
+      <c r="M29" s="13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="14.75" customHeight="1">
+      <c r="A30" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" s="9">
+        <v>120238</v>
+      </c>
+      <c r="I30" s="9">
+        <v>489581</v>
+      </c>
+      <c r="J30" s="9">
+        <v>52.392972999999998</v>
+      </c>
+      <c r="K30" s="9">
+        <v>4.876512</v>
+      </c>
+      <c r="L30" s="9">
+        <v>1</v>
+      </c>
+      <c r="M30" s="13">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="14.75" customHeight="1">
+      <c r="A31" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H31" s="9">
+        <v>122596</v>
+      </c>
+      <c r="I31" s="9">
+        <v>487972</v>
+      </c>
+      <c r="J31" s="9">
+        <v>52.378661000000001</v>
+      </c>
+      <c r="K31" s="9">
+        <v>4.9113069999999999</v>
+      </c>
+      <c r="L31" s="9">
+        <v>1</v>
+      </c>
+      <c r="M31" s="13">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.51180599999999998"/>

</xml_diff>